<commit_message>
Went through the whole project to fixes a couple of defects.
</commit_message>
<xml_diff>
--- a/src/test/java/ApachePOI/Resources/ApacheExcel2.xlsx
+++ b/src/test/java/ApachePOI/Resources/ApacheExcel2.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\berkg\IdeaProjects\Cucumber\src\test\java\ApachePOI\Resources\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ragip\IdeaProjects\Us_Batch7_Cucumber\src\test\java\ApachePOI\Resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1B4A9978-9628-42B4-A46E-E7A06CFF4E40}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8595D97C-3C98-4BAF-9150-C494AAD4E4FB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="2190" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -52,52 +52,52 @@
     <t>End</t>
   </si>
   <si>
-    <t>US B7 1</t>
-  </si>
-  <si>
-    <t>US B7 2</t>
-  </si>
-  <si>
-    <t>US B7 3</t>
-  </si>
-  <si>
-    <t>US B7 4</t>
-  </si>
-  <si>
-    <t>US B7 5</t>
-  </si>
-  <si>
-    <t>US B7 6</t>
-  </si>
-  <si>
-    <t>US B7 7</t>
-  </si>
-  <si>
-    <t>US B7 8</t>
-  </si>
-  <si>
-    <t>b7_1</t>
-  </si>
-  <si>
-    <t>b7_2</t>
-  </si>
-  <si>
-    <t>b7_3</t>
-  </si>
-  <si>
-    <t>b7_4</t>
-  </si>
-  <si>
-    <t>b7_5</t>
-  </si>
-  <si>
-    <t>b7_6</t>
-  </si>
-  <si>
-    <t>b7_7</t>
-  </si>
-  <si>
-    <t>b7_8</t>
+    <t>Us Batch 7 1</t>
+  </si>
+  <si>
+    <t>Us Batch 7 2</t>
+  </si>
+  <si>
+    <t>Us Batch 7 3</t>
+  </si>
+  <si>
+    <t>Us Batch 7 4</t>
+  </si>
+  <si>
+    <t>Us Batch 7 5</t>
+  </si>
+  <si>
+    <t>Us Batch 7 6</t>
+  </si>
+  <si>
+    <t>Us Batch 7 7</t>
+  </si>
+  <si>
+    <t>Us Batch 7 8</t>
+  </si>
+  <si>
+    <t>ub71</t>
+  </si>
+  <si>
+    <t>ub72</t>
+  </si>
+  <si>
+    <t>ub73</t>
+  </si>
+  <si>
+    <t>ub74</t>
+  </si>
+  <si>
+    <t>ub75</t>
+  </si>
+  <si>
+    <t>ub76</t>
+  </si>
+  <si>
+    <t>ub77</t>
+  </si>
+  <si>
+    <t>ub78</t>
   </si>
 </sst>
 </file>
@@ -507,8 +507,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:B8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B13" sqref="B13"/>
+    <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>